<commit_message>
Implement enemy name generator.
Added some if debug logic.
</commit_message>
<xml_diff>
--- a/EnemyNames.xlsx
+++ b/EnemyNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altam\OneDrive\Documents\GIT\MechsAndMagesPrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92B9714-2376-4A1C-B516-4EC55221F1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15EC39D-93B4-4731-B056-6BB218C1527A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B57CD62C-486C-46DF-9F94-EC78F24620D3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="139">
   <si>
     <t>The</t>
   </si>
@@ -91,15 +91,9 @@
     <t>Regiment</t>
   </si>
   <si>
-    <t>Throng</t>
-  </si>
-  <si>
     <t>Horde</t>
   </si>
   <si>
-    <t>Multitude</t>
-  </si>
-  <si>
     <t>Squadron</t>
   </si>
   <si>
@@ -127,9 +121,6 @@
     <t>Organization</t>
   </si>
   <si>
-    <t>Crusaders</t>
-  </si>
-  <si>
     <t>Swarm</t>
   </si>
   <si>
@@ -154,9 +145,6 @@
     <t>Flood</t>
   </si>
   <si>
-    <t>Holistic</t>
-  </si>
-  <si>
     <t>Holy</t>
   </si>
   <si>
@@ -211,9 +199,6 @@
     <t>Resolute</t>
   </si>
   <si>
-    <t>Guided</t>
-  </si>
-  <si>
     <t>Bright</t>
   </si>
   <si>
@@ -232,12 +217,6 @@
     <t>Evolved</t>
   </si>
   <si>
-    <t>Excelled</t>
-  </si>
-  <si>
-    <t>Transcended</t>
-  </si>
-  <si>
     <t>Bold</t>
   </si>
   <si>
@@ -286,18 +265,9 @@
     <t>Platoon</t>
   </si>
   <si>
-    <t>Outsiders</t>
-  </si>
-  <si>
-    <t>Guardians</t>
-  </si>
-  <si>
     <t>Wheeping</t>
   </si>
   <si>
-    <t>Looming</t>
-  </si>
-  <si>
     <t>Unwavering</t>
   </si>
   <si>
@@ -349,9 +319,6 @@
     <t>With</t>
   </si>
   <si>
-    <t>Bound By</t>
-  </si>
-  <si>
     <t>Loyal To</t>
   </si>
   <si>
@@ -370,9 +337,6 @@
     <t>Mech</t>
   </si>
   <si>
-    <t>Droid</t>
-  </si>
-  <si>
     <t>Neutral</t>
   </si>
   <si>
@@ -382,9 +346,6 @@
     <t>Place</t>
   </si>
   <si>
-    <t>Co-operative</t>
-  </si>
-  <si>
     <t>United</t>
   </si>
   <si>
@@ -394,32 +355,110 @@
     <t>Dedicated</t>
   </si>
   <si>
-    <t>Peaceful</t>
-  </si>
-  <si>
-    <t>Archaic</t>
-  </si>
-  <si>
-    <t>Supported</t>
-  </si>
-  <si>
     <t>Assisting</t>
   </si>
   <si>
-    <t>Mediating</t>
-  </si>
-  <si>
-    <t>Guarding</t>
-  </si>
-  <si>
-    <t>Backup</t>
+    <t>Protective</t>
+  </si>
+  <si>
+    <t>Federated</t>
+  </si>
+  <si>
+    <t>Long-standing</t>
+  </si>
+  <si>
+    <t>Impartial</t>
+  </si>
+  <si>
+    <t>Even-handed</t>
+  </si>
+  <si>
+    <t>Innocuous</t>
+  </si>
+  <si>
+    <t>Anodyne</t>
+  </si>
+  <si>
+    <t>Harmonious</t>
+  </si>
+  <si>
+    <t>Fighting For</t>
+  </si>
+  <si>
+    <t>Standing With</t>
+  </si>
+  <si>
+    <t>Sent By</t>
+  </si>
+  <si>
+    <t>Formed In</t>
+  </si>
+  <si>
+    <t>Pious</t>
+  </si>
+  <si>
+    <t>Borg</t>
+  </si>
+  <si>
+    <t>Guardianship</t>
+  </si>
+  <si>
+    <t>Brotherhood</t>
+  </si>
+  <si>
+    <t>Crusade</t>
+  </si>
+  <si>
+    <t>Compartment</t>
+  </si>
+  <si>
+    <t>Opposing</t>
+  </si>
+  <si>
+    <t>In Conflict With</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revolting Against </t>
+  </si>
+  <si>
+    <t>Standing Against</t>
+  </si>
+  <si>
+    <t>Viscious</t>
+  </si>
+  <si>
+    <t>Luminous</t>
+  </si>
+  <si>
+    <t>Transcendent</t>
+  </si>
+  <si>
+    <t>Threatening</t>
+  </si>
+  <si>
+    <t>Bound To</t>
+  </si>
+  <si>
+    <t>Sworn Against</t>
+  </si>
+  <si>
+    <t>Siding With</t>
+  </si>
+  <si>
+    <t>Siding Against</t>
+  </si>
+  <si>
+    <t>Whivyn</t>
+  </si>
+  <si>
+    <t>Lischering</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,16 +466,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -444,15 +497,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,15 +539,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{181E3FF9-E195-4ED2-801B-5F1FCDBC8A4F}" name="Table2" displayName="Table2" ref="A1:I43" totalsRowShown="0">
-  <autoFilter ref="A1:I43" xr:uid="{181E3FF9-E195-4ED2-801B-5F1FCDBC8A4F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{181E3FF9-E195-4ED2-801B-5F1FCDBC8A4F}" name="Table2" displayName="Table2" ref="A1:I1048576" totalsRowShown="0">
+  <autoFilter ref="A1:I1048576" xr:uid="{181E3FF9-E195-4ED2-801B-5F1FCDBC8A4F}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C0AA8EEE-480C-4F3F-AB0E-33FF99DF8AA9}" name="Pre"/>
-    <tableColumn id="2" xr3:uid="{6A4FD79A-4987-4136-AE87-227C17B3A6EE}" name="Mage"/>
-    <tableColumn id="3" xr3:uid="{452886E3-3CA4-405D-B167-58D91647BCF3}" name="Necro"/>
+    <tableColumn id="2" xr3:uid="{6A4FD79A-4987-4136-AE87-227C17B3A6EE}" name="Neutral"/>
+    <tableColumn id="3" xr3:uid="{452886E3-3CA4-405D-B167-58D91647BCF3}" name="Borg"/>
     <tableColumn id="4" xr3:uid="{EEF77041-B170-4ADE-848B-3DC8D476AA19}" name="Mech"/>
-    <tableColumn id="5" xr3:uid="{FE35FA3E-E335-4596-9908-07B15C0C311B}" name="Droid"/>
-    <tableColumn id="6" xr3:uid="{4FDB05EA-0C14-41AA-8206-8F1D873DC6B3}" name="Neutral"/>
+    <tableColumn id="5" xr3:uid="{FE35FA3E-E335-4596-9908-07B15C0C311B}" name="Mage"/>
+    <tableColumn id="6" xr3:uid="{4FDB05EA-0C14-41AA-8206-8F1D873DC6B3}" name="Necro"/>
     <tableColumn id="7" xr3:uid="{FA7B6ADD-83B7-4167-99C3-52886A58D0B6}" name="Collective" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{D0D57E90-7993-46B4-AAEF-57A27D8BEE9B}" name="Post"/>
     <tableColumn id="9" xr3:uid="{DFE945BC-954D-4DA3-BBFB-33F46C488B82}" name="Place"/>
@@ -789,52 +853,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B424E1-C266-42E9-996C-1B79EA99026A}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" t="s">
-        <v>112</v>
+        <v>100</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="G1" t="s">
         <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="I1" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -842,443 +906,480 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" t="s">
-        <v>115</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="I2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" t="s">
-        <v>116</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="I3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" t="s">
-        <v>124</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" t="s">
-        <v>123</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="I5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="I6" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" t="s">
-        <v>117</v>
+      <c r="E7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="I7" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" t="s">
-        <v>118</v>
+        <v>105</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="I8" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" t="s">
-        <v>119</v>
+        <v>114</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>83</v>
+        <v>124</v>
+      </c>
+      <c r="H9" t="s">
+        <v>106</v>
       </c>
       <c r="I9" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" t="s">
-        <v>120</v>
+        <v>109</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="H10" t="s">
+        <v>115</v>
+      </c>
       <c r="I10" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" t="s">
-        <v>121</v>
+        <v>110</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
+      </c>
+      <c r="H11" t="s">
+        <v>116</v>
+      </c>
+      <c r="I11" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" t="s">
-        <v>122</v>
+      <c r="E12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I12" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" t="s">
-        <v>125</v>
+      <c r="E13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G14" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="H14" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H15" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G16" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G17" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G18" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G19" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G20" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="H20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G21" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G25" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G26" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G27" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G28" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G29" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G30" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G31" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G32" s="1" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G32" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G35" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G36" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G37" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G38" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G39" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G40" s="1" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G41" s="1" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G42" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G43" s="1" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started adding game loop logic for selecting nodes.
</commit_message>
<xml_diff>
--- a/EnemyNames.xlsx
+++ b/EnemyNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altam\OneDrive\Documents\GIT\MechsAndMagesPrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15EC39D-93B4-4731-B056-6BB218C1527A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63FF4B3-DC37-4CBD-820C-BB482EEF550B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B57CD62C-486C-46DF-9F94-EC78F24620D3}"/>
   </bookViews>
@@ -169,9 +169,6 @@
     <t>Revolting</t>
   </si>
   <si>
-    <t>Energised</t>
-  </si>
-  <si>
     <t>Saprked</t>
   </si>
   <si>
@@ -452,6 +449,9 @@
   </si>
   <si>
     <t>Lischering</t>
+  </si>
+  <si>
+    <t>Entropic</t>
   </si>
 </sst>
 </file>
@@ -856,7 +856,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,31 +874,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="G1" t="s">
         <v>8</v>
       </c>
       <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
         <v>101</v>
-      </c>
-      <c r="I1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -906,16 +906,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>1</v>
@@ -924,21 +924,21 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>43</v>
@@ -953,21 +953,21 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>37</v>
@@ -979,21 +979,21 @@
         <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>38</v>
@@ -1005,215 +1005,215 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>39</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1221,7 +1221,7 @@
         <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1229,7 +1229,7 @@
         <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1237,7 +1237,7 @@
         <v>13</v>
       </c>
       <c r="H16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.25">
@@ -1245,7 +1245,7 @@
         <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="7:8" x14ac:dyDescent="0.25">
@@ -1253,7 +1253,7 @@
         <v>15</v>
       </c>
       <c r="H18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="7:8" x14ac:dyDescent="0.25">
@@ -1261,15 +1261,15 @@
         <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="7:8" x14ac:dyDescent="0.25">
@@ -1324,7 +1324,7 @@
     </row>
     <row r="31" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G31" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="7:8" x14ac:dyDescent="0.25">
@@ -1369,17 +1369,17 @@
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G40" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G41" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G42" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>